<commit_message>
andamento do product backlog
</commit_message>
<xml_diff>
--- a/documentação/product_backlog.xlsx
+++ b/documentação/product_backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Desktop\projeto BandTec\TI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micazev/paiotnela/documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7368930-5920-4B4F-B714-64FDDCF95540}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B7807A-071E-BE4A-A2A7-72F99D91B3F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1560B7A6-87AF-4E19-B796-FA907A36D599}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{1560B7A6-87AF-4E19-B796-FA907A36D599}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1055,7 +1055,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1148,9 +1148,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1160,23 +1157,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="20% - Ênfase1" xfId="2" builtinId="30"/>
-    <cellStyle name="60% - Ênfase1" xfId="3" builtinId="32"/>
-    <cellStyle name="Ênfase1" xfId="1" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1198,7 +1204,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1496,21 +1502,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB73C86A-86DA-463D-9718-431C94514CCD}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -1528,7 +1534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1536,14 +1542,14 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="44" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="10">
@@ -1556,12 +1562,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="34"/>
       <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="10">
@@ -1574,12 +1580,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="34"/>
       <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="44" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="10">
@@ -1592,12 +1598,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="34"/>
       <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="44" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="10">
@@ -1610,12 +1616,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="34"/>
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="10">
@@ -1628,12 +1634,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="34"/>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="44" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="10">
@@ -1646,7 +1652,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="34"/>
       <c r="B9" s="10" t="s">
         <v>10</v>
@@ -1664,12 +1670,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="34"/>
       <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="44" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="10">
@@ -1682,12 +1688,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="34"/>
       <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="44" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="10">
@@ -1700,12 +1706,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="34"/>
       <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="44" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="10">
@@ -1718,7 +1724,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="34"/>
       <c r="B13" s="10" t="s">
         <v>14</v>
@@ -1736,12 +1742,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="34"/>
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="44" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="10">
@@ -1754,12 +1760,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="34"/>
       <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="44" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="10">
@@ -1772,7 +1778,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="34"/>
       <c r="B16" s="10" t="s">
         <v>30</v>
@@ -1790,7 +1796,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="34"/>
       <c r="B17" s="10" t="s">
         <v>31</v>
@@ -1808,7 +1814,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="34"/>
       <c r="B18" s="10" t="s">
         <v>32</v>
@@ -1826,7 +1832,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="34"/>
       <c r="B19" s="10" t="s">
         <v>33</v>
@@ -1844,7 +1850,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="34"/>
       <c r="B20" s="10" t="s">
         <v>34</v>
@@ -1862,7 +1868,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="34"/>
       <c r="B21" s="10" t="s">
         <v>35</v>
@@ -1880,7 +1886,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="34"/>
       <c r="B22" s="10" t="s">
         <v>44</v>
@@ -1898,7 +1904,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="34"/>
       <c r="B23" s="10" t="s">
         <v>45</v>
@@ -1916,7 +1922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="34"/>
       <c r="B24" s="10" t="s">
         <v>68</v>
@@ -1934,7 +1940,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="4.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1942,7 +1948,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="35" t="s">
         <v>147</v>
       </c>
@@ -1962,7 +1968,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="10" t="s">
         <v>73</v>
@@ -1980,7 +1986,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="34"/>
       <c r="B28" s="10" t="s">
         <v>74</v>
@@ -1998,7 +2004,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="34"/>
       <c r="B29" s="10" t="s">
         <v>75</v>
@@ -2016,7 +2022,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="34"/>
       <c r="B30" s="10" t="s">
         <v>76</v>
@@ -2034,7 +2040,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="3.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2042,7 +2048,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
         <v>87</v>
       </c>
@@ -2062,7 +2068,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="31"/>
       <c r="B33" s="10" t="s">
         <v>72</v>
@@ -2080,7 +2086,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="31"/>
       <c r="B34" s="10" t="s">
         <v>73</v>
@@ -2098,7 +2104,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="31"/>
       <c r="B35" s="10" t="s">
         <v>74</v>
@@ -2116,7 +2122,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="31"/>
       <c r="B36" s="10" t="s">
         <v>75</v>
@@ -2134,7 +2140,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="31"/>
       <c r="B37" s="10" t="s">
         <v>76</v>
@@ -2152,7 +2158,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="32"/>
       <c r="B38" s="10" t="s">
         <v>94</v>
@@ -2170,7 +2176,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="3.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2178,7 +2184,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
         <v>96</v>
       </c>
@@ -2198,7 +2204,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="34"/>
       <c r="B41" s="10" t="s">
         <v>5</v>
@@ -2216,7 +2222,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="34"/>
       <c r="B42" s="10" t="s">
         <v>6</v>
@@ -2234,7 +2240,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="34"/>
       <c r="B43" s="10" t="s">
         <v>7</v>
@@ -2252,7 +2258,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="34"/>
       <c r="B44" s="10" t="s">
         <v>72</v>
@@ -2270,7 +2276,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="34"/>
       <c r="B45" s="10" t="s">
         <v>73</v>
@@ -2288,7 +2294,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="4.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2296,7 +2302,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="30" t="s">
         <v>113</v>
       </c>
@@ -2316,7 +2322,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="31"/>
       <c r="B48" s="26" t="s">
         <v>4</v>
@@ -2334,7 +2340,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="31"/>
       <c r="B49" s="26" t="s">
         <v>5</v>
@@ -2352,7 +2358,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="31"/>
       <c r="B50" s="26" t="s">
         <v>6</v>
@@ -2370,7 +2376,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="31"/>
       <c r="B51" s="26" t="s">
         <v>7</v>
@@ -2388,7 +2394,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="31"/>
       <c r="B52" s="26" t="s">
         <v>8</v>
@@ -2406,7 +2412,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="31"/>
       <c r="B53" s="26" t="s">
         <v>9</v>
@@ -2424,7 +2430,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="32"/>
       <c r="B54" s="26" t="s">
         <v>10</v>
@@ -2459,30 +2465,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5994EBB2-7D56-4B66-AE3B-20C2BD3DC2FB}">
   <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="0.6640625" customWidth="1"/>
     <col min="5" max="5" width="61.33203125" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F1" s="40" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F1" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="G1" s="41"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G1" s="43"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>114</v>
@@ -2490,7 +2496,7 @@
       <c r="C2" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="42"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="6" t="s">
         <v>116</v>
       </c>
@@ -2507,28 +2513,28 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="3.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="36"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="37">
-        <v>5</v>
-      </c>
-      <c r="D4" s="36"/>
+      <c r="C4" s="36">
+        <v>5</v>
+      </c>
+      <c r="D4" s="40"/>
       <c r="E4" s="20" t="s">
         <v>123</v>
       </c>
@@ -2539,11 +2545,11 @@
       </c>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="31"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="20" t="s">
         <v>124</v>
       </c>
@@ -2554,11 +2560,11 @@
       </c>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="31"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="36"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="20" t="s">
         <v>125</v>
       </c>
@@ -2569,15 +2575,15 @@
       </c>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="31"/>
-      <c r="B7" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="37">
+      <c r="B7" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="36">
         <v>3</v>
       </c>
-      <c r="D7" s="36"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="20" t="s">
         <v>126</v>
       </c>
@@ -2588,11 +2594,11 @@
       </c>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="31"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="36"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="20" t="s">
         <v>127</v>
       </c>
@@ -2603,11 +2609,11 @@
       </c>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="31"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="20" t="s">
         <v>128</v>
       </c>
@@ -2618,11 +2624,11 @@
       </c>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="31"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="36"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="20" t="s">
         <v>129</v>
       </c>
@@ -2633,15 +2639,15 @@
       </c>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="31"/>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="36">
         <v>3</v>
       </c>
-      <c r="D11" s="36"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="20" t="s">
         <v>126</v>
       </c>
@@ -2652,11 +2658,11 @@
       </c>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="31"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="20" t="s">
         <v>127</v>
       </c>
@@ -2667,11 +2673,11 @@
       </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="31"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="20" t="s">
         <v>128</v>
       </c>
@@ -2682,11 +2688,11 @@
       </c>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="31"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="36"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="20" t="s">
         <v>129</v>
       </c>
@@ -2697,15 +2703,15 @@
       </c>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="31"/>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="36">
         <v>3</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="40"/>
       <c r="E15" s="20" t="s">
         <v>126</v>
       </c>
@@ -2716,11 +2722,11 @@
       </c>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="31"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="40"/>
       <c r="E16" s="20" t="s">
         <v>127</v>
       </c>
@@ -2731,11 +2737,11 @@
       </c>
       <c r="I16" s="14"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="31"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="20" t="s">
         <v>128</v>
       </c>
@@ -2746,11 +2752,11 @@
       </c>
       <c r="I17" s="14"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="31"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="36"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="20" t="s">
         <v>129</v>
       </c>
@@ -2761,15 +2767,15 @@
       </c>
       <c r="I18" s="14"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="31"/>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="37">
+      <c r="C19" s="36">
         <v>3</v>
       </c>
-      <c r="D19" s="36"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="20" t="s">
         <v>126</v>
       </c>
@@ -2780,11 +2786,11 @@
       </c>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="31"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="20" t="s">
         <v>127</v>
       </c>
@@ -2795,11 +2801,11 @@
       </c>
       <c r="I20" s="14"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="31"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="20" t="s">
         <v>128</v>
       </c>
@@ -2810,11 +2816,11 @@
       </c>
       <c r="I21" s="14"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="31"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="36"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="40"/>
       <c r="E22" s="20" t="s">
         <v>129</v>
       </c>
@@ -2825,15 +2831,15 @@
       </c>
       <c r="I22" s="14"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="31"/>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="36">
         <v>3</v>
       </c>
-      <c r="D23" s="36"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="20" t="s">
         <v>126</v>
       </c>
@@ -2844,11 +2850,11 @@
       </c>
       <c r="I23" s="14"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="31"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="36"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="20" t="s">
         <v>127</v>
       </c>
@@ -2859,11 +2865,11 @@
       </c>
       <c r="I24" s="14"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="31"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="36"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="20" t="s">
         <v>128</v>
       </c>
@@ -2874,11 +2880,11 @@
       </c>
       <c r="I25" s="14"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="31"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="36"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="40"/>
       <c r="E26" s="20" t="s">
         <v>129</v>
       </c>
@@ -2889,15 +2895,15 @@
       </c>
       <c r="I26" s="14"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="31"/>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="37">
+      <c r="C27" s="36">
         <v>3</v>
       </c>
-      <c r="D27" s="36"/>
+      <c r="D27" s="40"/>
       <c r="E27" s="20" t="s">
         <v>130</v>
       </c>
@@ -2908,11 +2914,11 @@
       </c>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="31"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="36"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="40"/>
       <c r="E28" s="20" t="s">
         <v>131</v>
       </c>
@@ -2923,11 +2929,11 @@
       </c>
       <c r="I28" s="14"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="31"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="36"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="40"/>
       <c r="E29" s="20" t="s">
         <v>132</v>
       </c>
@@ -2938,15 +2944,15 @@
       </c>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="31"/>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="37">
-        <v>5</v>
-      </c>
-      <c r="D30" s="36"/>
+      <c r="C30" s="36">
+        <v>5</v>
+      </c>
+      <c r="D30" s="40"/>
       <c r="E30" s="20" t="s">
         <v>126</v>
       </c>
@@ -2957,11 +2963,11 @@
       </c>
       <c r="I30" s="14"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="31"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="36"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="40"/>
       <c r="E31" s="20" t="s">
         <v>133</v>
       </c>
@@ -2972,11 +2978,11 @@
       </c>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="31"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="20" t="s">
         <v>134</v>
       </c>
@@ -2987,15 +2993,15 @@
       </c>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="31"/>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="37">
-        <v>5</v>
-      </c>
-      <c r="D33" s="36"/>
+      <c r="C33" s="36">
+        <v>5</v>
+      </c>
+      <c r="D33" s="40"/>
       <c r="E33" s="20" t="s">
         <v>136</v>
       </c>
@@ -3006,11 +3012,11 @@
       </c>
       <c r="I33" s="14"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="31"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="40"/>
       <c r="E34" s="20" t="s">
         <v>133</v>
       </c>
@@ -3021,11 +3027,11 @@
       </c>
       <c r="I34" s="14"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="31"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="36"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="40"/>
       <c r="E35" s="20" t="s">
         <v>135</v>
       </c>
@@ -3036,15 +3042,15 @@
       </c>
       <c r="I35" s="14"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="31"/>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="37">
-        <v>5</v>
-      </c>
-      <c r="D36" s="36"/>
+      <c r="C36" s="36">
+        <v>5</v>
+      </c>
+      <c r="D36" s="40"/>
       <c r="E36" s="20" t="s">
         <v>137</v>
       </c>
@@ -3055,11 +3061,11 @@
       </c>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="31"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="36"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="40"/>
       <c r="E37" s="20" t="s">
         <v>138</v>
       </c>
@@ -3070,11 +3076,11 @@
       </c>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="31"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="36"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="40"/>
       <c r="E38" s="20" t="s">
         <v>139</v>
       </c>
@@ -3085,15 +3091,15 @@
       </c>
       <c r="I38" s="14"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="37">
+      <c r="C39" s="36">
         <v>1</v>
       </c>
-      <c r="D39" s="36"/>
+      <c r="D39" s="40"/>
       <c r="E39" s="20" t="s">
         <v>140</v>
       </c>
@@ -3104,11 +3110,11 @@
       </c>
       <c r="I39" s="14"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="31"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="36"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="40"/>
       <c r="E40" s="20" t="s">
         <v>141</v>
       </c>
@@ -3119,15 +3125,15 @@
       </c>
       <c r="I40" s="14"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="31"/>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="37">
-        <v>5</v>
-      </c>
-      <c r="D41" s="36"/>
+      <c r="C41" s="36">
+        <v>5</v>
+      </c>
+      <c r="D41" s="40"/>
       <c r="E41" s="20" t="s">
         <v>142</v>
       </c>
@@ -3138,11 +3144,11 @@
       </c>
       <c r="I41" s="14"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="31"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="40"/>
       <c r="E42" s="20" t="s">
         <v>143</v>
       </c>
@@ -3153,11 +3159,11 @@
       </c>
       <c r="I42" s="14"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="31"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="40"/>
       <c r="E43" s="20" t="s">
         <v>146</v>
       </c>
@@ -3168,11 +3174,11 @@
       </c>
       <c r="I43" s="14"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="31"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="36"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="40"/>
       <c r="E44" s="20" t="s">
         <v>144</v>
       </c>
@@ -3183,15 +3189,15 @@
       </c>
       <c r="I44" s="14"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="31"/>
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="37">
-        <v>5</v>
-      </c>
-      <c r="D45" s="36"/>
+      <c r="C45" s="36">
+        <v>5</v>
+      </c>
+      <c r="D45" s="40"/>
       <c r="E45" s="20" t="s">
         <v>145</v>
       </c>
@@ -3202,11 +3208,11 @@
       </c>
       <c r="I45" s="14"/>
     </row>
-    <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="31"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="36"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="40"/>
       <c r="E46" s="20" t="s">
         <v>150</v>
       </c>
@@ -3217,11 +3223,11 @@
       </c>
       <c r="I46" s="14"/>
     </row>
-    <row r="47" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="31"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="36"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="40"/>
       <c r="E47" s="20" t="s">
         <v>151</v>
       </c>
@@ -3232,15 +3238,15 @@
       </c>
       <c r="I47" s="14"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="31"/>
-      <c r="B48" s="37" t="s">
+      <c r="B48" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="37">
-        <v>5</v>
-      </c>
-      <c r="D48" s="36"/>
+      <c r="C48" s="36">
+        <v>5</v>
+      </c>
+      <c r="D48" s="40"/>
       <c r="E48" s="20" t="s">
         <v>152</v>
       </c>
@@ -3251,11 +3257,11 @@
       </c>
       <c r="I48" s="14"/>
     </row>
-    <row r="49" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="31"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="36"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="40"/>
       <c r="E49" s="20" t="s">
         <v>153</v>
       </c>
@@ -3266,11 +3272,11 @@
       </c>
       <c r="I49" s="14"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="31"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="36"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="40"/>
       <c r="E50" s="20" t="s">
         <v>154</v>
       </c>
@@ -3281,15 +3287,15 @@
       </c>
       <c r="I50" s="14"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="31"/>
-      <c r="B51" s="37" t="s">
+      <c r="B51" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="37">
+      <c r="C51" s="36">
         <v>4</v>
       </c>
-      <c r="D51" s="36"/>
+      <c r="D51" s="40"/>
       <c r="E51" s="20" t="s">
         <v>155</v>
       </c>
@@ -3300,11 +3306,11 @@
       </c>
       <c r="I51" s="14"/>
     </row>
-    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="31"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="36"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="40"/>
       <c r="E52" s="20" t="s">
         <v>156</v>
       </c>
@@ -3315,11 +3321,11 @@
       </c>
       <c r="I52" s="14"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="31"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="36"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="40"/>
       <c r="E53" s="20" t="s">
         <v>157</v>
       </c>
@@ -3330,15 +3336,15 @@
       </c>
       <c r="I53" s="14"/>
     </row>
-    <row r="54" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="31"/>
-      <c r="B54" s="37" t="s">
+      <c r="B54" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="37">
+      <c r="C54" s="36">
         <v>4</v>
       </c>
-      <c r="D54" s="36"/>
+      <c r="D54" s="40"/>
       <c r="E54" s="20" t="s">
         <v>158</v>
       </c>
@@ -3349,11 +3355,11 @@
       </c>
       <c r="I54" s="14"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="31"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="36"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="40"/>
       <c r="E55" s="20" t="s">
         <v>159</v>
       </c>
@@ -3364,11 +3370,11 @@
       </c>
       <c r="I55" s="14"/>
     </row>
-    <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="31"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="36"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="40"/>
       <c r="E56" s="20" t="s">
         <v>161</v>
       </c>
@@ -3381,15 +3387,15 @@
       </c>
       <c r="I56" s="14"/>
     </row>
-    <row r="57" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="31"/>
-      <c r="B57" s="37" t="s">
+      <c r="B57" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C57" s="37">
+      <c r="C57" s="36">
         <v>4</v>
       </c>
-      <c r="D57" s="36"/>
+      <c r="D57" s="40"/>
       <c r="E57" s="20" t="s">
         <v>162</v>
       </c>
@@ -3400,11 +3406,11 @@
       </c>
       <c r="I57" s="14"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="31"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="36"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="40"/>
       <c r="E58" s="20" t="s">
         <v>163</v>
       </c>
@@ -3415,11 +3421,11 @@
       </c>
       <c r="I58" s="14"/>
     </row>
-    <row r="59" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="31"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="36"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="40"/>
       <c r="E59" s="20" t="s">
         <v>164</v>
       </c>
@@ -3430,15 +3436,15 @@
       </c>
       <c r="I59" s="14"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="31"/>
-      <c r="B60" s="37" t="s">
+      <c r="B60" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C60" s="37">
+      <c r="C60" s="36">
         <v>4</v>
       </c>
-      <c r="D60" s="36"/>
+      <c r="D60" s="40"/>
       <c r="E60" s="20" t="s">
         <v>165</v>
       </c>
@@ -3449,11 +3455,11 @@
       </c>
       <c r="I60" s="14"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="31"/>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="36"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="40"/>
       <c r="E61" s="20" t="s">
         <v>166</v>
       </c>
@@ -3464,11 +3470,11 @@
       </c>
       <c r="I61" s="14"/>
     </row>
-    <row r="62" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="31"/>
-      <c r="B62" s="39"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="36"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="40"/>
       <c r="E62" s="20" t="s">
         <v>167</v>
       </c>
@@ -3479,15 +3485,15 @@
       </c>
       <c r="I62" s="14"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="31"/>
-      <c r="B63" s="37" t="s">
+      <c r="B63" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C63" s="37">
-        <v>5</v>
-      </c>
-      <c r="D63" s="36"/>
+      <c r="C63" s="36">
+        <v>5</v>
+      </c>
+      <c r="D63" s="40"/>
       <c r="E63" s="20" t="s">
         <v>168</v>
       </c>
@@ -3498,11 +3504,11 @@
       </c>
       <c r="I63" s="14"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="31"/>
-      <c r="B64" s="38"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="36"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="40"/>
       <c r="E64" s="20" t="s">
         <v>169</v>
       </c>
@@ -3513,11 +3519,11 @@
       </c>
       <c r="I64" s="14"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="31"/>
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="36"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="40"/>
       <c r="E65" s="20" t="s">
         <v>170</v>
       </c>
@@ -3528,15 +3534,15 @@
       </c>
       <c r="I65" s="14"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="31"/>
-      <c r="B66" s="37" t="s">
+      <c r="B66" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C66" s="37">
-        <v>5</v>
-      </c>
-      <c r="D66" s="36"/>
+      <c r="C66" s="36">
+        <v>5</v>
+      </c>
+      <c r="D66" s="40"/>
       <c r="E66" s="20" t="s">
         <v>171</v>
       </c>
@@ -3547,11 +3553,11 @@
       </c>
       <c r="I66" s="14"/>
     </row>
-    <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="31"/>
-      <c r="B67" s="38"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="36"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="40"/>
       <c r="E67" s="20" t="s">
         <v>172</v>
       </c>
@@ -3562,11 +3568,11 @@
       </c>
       <c r="I67" s="14"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="31"/>
-      <c r="B68" s="39"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="36"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="40"/>
       <c r="E68" s="20" t="s">
         <v>173</v>
       </c>
@@ -3577,15 +3583,15 @@
       </c>
       <c r="I68" s="14"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="31"/>
-      <c r="B69" s="37" t="s">
+      <c r="B69" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C69" s="37">
+      <c r="C69" s="36">
         <v>2</v>
       </c>
-      <c r="D69" s="36"/>
+      <c r="D69" s="40"/>
       <c r="E69" s="20" t="s">
         <v>174</v>
       </c>
@@ -3596,11 +3602,11 @@
       </c>
       <c r="I69" s="14"/>
     </row>
-    <row r="70" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="31"/>
-      <c r="B70" s="38"/>
-      <c r="C70" s="38"/>
-      <c r="D70" s="36"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="40"/>
       <c r="E70" s="20" t="s">
         <v>175</v>
       </c>
@@ -3611,11 +3617,11 @@
       </c>
       <c r="I70" s="14"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="31"/>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="36"/>
+      <c r="B71" s="38"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="40"/>
       <c r="E71" s="20" t="s">
         <v>176</v>
       </c>
@@ -3626,15 +3632,15 @@
       </c>
       <c r="I71" s="14"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="31"/>
-      <c r="B72" s="37" t="s">
+      <c r="B72" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C72" s="37">
+      <c r="C72" s="36">
         <v>2</v>
       </c>
-      <c r="D72" s="36"/>
+      <c r="D72" s="40"/>
       <c r="E72" s="20" t="s">
         <v>177</v>
       </c>
@@ -3645,11 +3651,11 @@
       </c>
       <c r="I72" s="14"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="31"/>
-      <c r="B73" s="38"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="36"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="40"/>
       <c r="E73" s="20" t="s">
         <v>178</v>
       </c>
@@ -3660,11 +3666,11 @@
       </c>
       <c r="I73" s="14"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="32"/>
-      <c r="B74" s="39"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="36"/>
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="40"/>
       <c r="E74" s="20" t="s">
         <v>179</v>
       </c>
@@ -3675,28 +3681,28 @@
       </c>
       <c r="I74" s="14"/>
     </row>
-    <row r="75" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="36"/>
+      <c r="D75" s="40"/>
       <c r="E75" s="16"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
     </row>
-    <row r="76" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B76" s="37" t="s">
+      <c r="B76" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C76" s="37">
-        <v>5</v>
-      </c>
-      <c r="D76" s="36"/>
+      <c r="C76" s="36">
+        <v>5</v>
+      </c>
+      <c r="D76" s="40"/>
       <c r="E76" s="20" t="s">
         <v>180</v>
       </c>
@@ -3707,11 +3713,11 @@
       </c>
       <c r="I76" s="14"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="31"/>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="36"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="40"/>
       <c r="E77" s="20" t="s">
         <v>182</v>
       </c>
@@ -3722,11 +3728,11 @@
       </c>
       <c r="I77" s="14"/>
     </row>
-    <row r="78" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="31"/>
-      <c r="B78" s="39"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="36"/>
+      <c r="B78" s="38"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="40"/>
       <c r="E78" s="20" t="s">
         <v>181</v>
       </c>
@@ -3737,15 +3743,15 @@
       </c>
       <c r="I78" s="14"/>
     </row>
-    <row r="79" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A79" s="31"/>
-      <c r="B79" s="37" t="s">
+      <c r="B79" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C79" s="37">
-        <v>5</v>
-      </c>
-      <c r="D79" s="36"/>
+      <c r="C79" s="36">
+        <v>5</v>
+      </c>
+      <c r="D79" s="40"/>
       <c r="E79" s="20" t="s">
         <v>183</v>
       </c>
@@ -3758,11 +3764,11 @@
         <v>235</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A80" s="31"/>
-      <c r="B80" s="38"/>
-      <c r="C80" s="38"/>
-      <c r="D80" s="36"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="40"/>
       <c r="E80" s="20" t="s">
         <v>184</v>
       </c>
@@ -3775,11 +3781,11 @@
         <v>235</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="31"/>
-      <c r="B81" s="39"/>
-      <c r="C81" s="39"/>
-      <c r="D81" s="36"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="40"/>
       <c r="E81" s="20" t="s">
         <v>185</v>
       </c>
@@ -3790,15 +3796,15 @@
       </c>
       <c r="I81" s="14"/>
     </row>
-    <row r="82" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="31"/>
-      <c r="B82" s="37" t="s">
+      <c r="B82" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="C82" s="37">
-        <v>5</v>
-      </c>
-      <c r="D82" s="36"/>
+      <c r="C82" s="36">
+        <v>5</v>
+      </c>
+      <c r="D82" s="40"/>
       <c r="E82" s="20" t="s">
         <v>186</v>
       </c>
@@ -3809,11 +3815,11 @@
       </c>
       <c r="I82" s="14"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="31"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="36"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="40"/>
       <c r="E83" s="20" t="s">
         <v>187</v>
       </c>
@@ -3824,11 +3830,11 @@
       </c>
       <c r="I83" s="14"/>
     </row>
-    <row r="84" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="31"/>
-      <c r="B84" s="39"/>
-      <c r="C84" s="39"/>
-      <c r="D84" s="36"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="40"/>
       <c r="E84" s="20" t="s">
         <v>188</v>
       </c>
@@ -3839,15 +3845,15 @@
       </c>
       <c r="I84" s="14"/>
     </row>
-    <row r="85" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="31"/>
-      <c r="B85" s="37" t="s">
+      <c r="B85" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C85" s="37">
-        <v>5</v>
-      </c>
-      <c r="D85" s="36"/>
+      <c r="C85" s="36">
+        <v>5</v>
+      </c>
+      <c r="D85" s="40"/>
       <c r="E85" s="20" t="s">
         <v>189</v>
       </c>
@@ -3858,11 +3864,11 @@
       </c>
       <c r="I85" s="14"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="31"/>
-      <c r="B86" s="38"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="36"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="40"/>
       <c r="E86" s="20" t="s">
         <v>190</v>
       </c>
@@ -3873,11 +3879,11 @@
       </c>
       <c r="I86" s="14"/>
     </row>
-    <row r="87" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="31"/>
-      <c r="B87" s="39"/>
-      <c r="C87" s="39"/>
-      <c r="D87" s="36"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="38"/>
+      <c r="D87" s="40"/>
       <c r="E87" s="20" t="s">
         <v>191</v>
       </c>
@@ -3888,15 +3894,15 @@
       </c>
       <c r="I87" s="14"/>
     </row>
-    <row r="88" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="31"/>
-      <c r="B88" s="37" t="s">
+      <c r="B88" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C88" s="37">
+      <c r="C88" s="36">
         <v>4</v>
       </c>
-      <c r="D88" s="36"/>
+      <c r="D88" s="40"/>
       <c r="E88" s="20" t="s">
         <v>192</v>
       </c>
@@ -3907,11 +3913,11 @@
       </c>
       <c r="I88" s="14"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="31"/>
-      <c r="B89" s="39"/>
-      <c r="C89" s="39"/>
-      <c r="D89" s="36"/>
+      <c r="B89" s="38"/>
+      <c r="C89" s="38"/>
+      <c r="D89" s="40"/>
       <c r="E89" s="20" t="s">
         <v>193</v>
       </c>
@@ -3922,28 +3928,28 @@
       </c>
       <c r="I89" s="14"/>
     </row>
-    <row r="90" spans="1:9" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="2.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
-      <c r="D90" s="36"/>
+      <c r="D90" s="40"/>
       <c r="E90" s="16"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
     </row>
-    <row r="91" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B91" s="37" t="s">
+      <c r="B91" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C91" s="37">
-        <v>5</v>
-      </c>
-      <c r="D91" s="36"/>
+      <c r="C91" s="36">
+        <v>5</v>
+      </c>
+      <c r="D91" s="40"/>
       <c r="E91" s="20" t="s">
         <v>194</v>
       </c>
@@ -3954,11 +3960,11 @@
       </c>
       <c r="I91" s="14"/>
     </row>
-    <row r="92" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="31"/>
-      <c r="B92" s="38"/>
-      <c r="C92" s="38"/>
-      <c r="D92" s="36"/>
+      <c r="B92" s="37"/>
+      <c r="C92" s="37"/>
+      <c r="D92" s="40"/>
       <c r="E92" s="20" t="s">
         <v>195</v>
       </c>
@@ -3969,11 +3975,11 @@
       </c>
       <c r="I92" s="14"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="31"/>
-      <c r="B93" s="38"/>
-      <c r="C93" s="38"/>
-      <c r="D93" s="36"/>
+      <c r="B93" s="37"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="40"/>
       <c r="E93" s="20" t="s">
         <v>196</v>
       </c>
@@ -3984,11 +3990,11 @@
       </c>
       <c r="I93" s="14"/>
     </row>
-    <row r="94" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="31"/>
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="36"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="38"/>
+      <c r="D94" s="40"/>
       <c r="E94" s="20" t="s">
         <v>197</v>
       </c>
@@ -3999,15 +4005,15 @@
       </c>
       <c r="I94" s="14"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="31"/>
-      <c r="B95" s="37" t="s">
+      <c r="B95" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C95" s="37">
-        <v>5</v>
-      </c>
-      <c r="D95" s="36"/>
+      <c r="C95" s="36">
+        <v>5</v>
+      </c>
+      <c r="D95" s="40"/>
       <c r="E95" s="20" t="s">
         <v>198</v>
       </c>
@@ -4018,11 +4024,11 @@
       </c>
       <c r="I95" s="14"/>
     </row>
-    <row r="96" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="31"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="36"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="40"/>
       <c r="E96" s="20" t="s">
         <v>199</v>
       </c>
@@ -4033,11 +4039,11 @@
       </c>
       <c r="I96" s="14"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="31"/>
-      <c r="B97" s="39"/>
-      <c r="C97" s="39"/>
-      <c r="D97" s="36"/>
+      <c r="B97" s="38"/>
+      <c r="C97" s="38"/>
+      <c r="D97" s="40"/>
       <c r="E97" s="20" t="s">
         <v>200</v>
       </c>
@@ -4048,15 +4054,15 @@
       </c>
       <c r="I97" s="14"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="31"/>
-      <c r="B98" s="37" t="s">
+      <c r="B98" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="37">
-        <v>5</v>
-      </c>
-      <c r="D98" s="36"/>
+      <c r="C98" s="36">
+        <v>5</v>
+      </c>
+      <c r="D98" s="40"/>
       <c r="E98" s="20" t="s">
         <v>201</v>
       </c>
@@ -4067,11 +4073,11 @@
       </c>
       <c r="I98" s="14"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="31"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="38"/>
-      <c r="D99" s="36"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="37"/>
+      <c r="D99" s="40"/>
       <c r="E99" s="20" t="s">
         <v>202</v>
       </c>
@@ -4082,11 +4088,11 @@
       </c>
       <c r="I99" s="14"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="31"/>
-      <c r="B100" s="38"/>
-      <c r="C100" s="38"/>
-      <c r="D100" s="36"/>
+      <c r="B100" s="37"/>
+      <c r="C100" s="37"/>
+      <c r="D100" s="40"/>
       <c r="E100" s="20" t="s">
         <v>203</v>
       </c>
@@ -4097,11 +4103,11 @@
       </c>
       <c r="I100" s="14"/>
     </row>
-    <row r="101" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="31"/>
-      <c r="B101" s="39"/>
-      <c r="C101" s="39"/>
-      <c r="D101" s="36"/>
+      <c r="B101" s="38"/>
+      <c r="C101" s="38"/>
+      <c r="D101" s="40"/>
       <c r="E101" s="20" t="s">
         <v>204</v>
       </c>
@@ -4112,15 +4118,15 @@
       </c>
       <c r="I101" s="14"/>
     </row>
-    <row r="102" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="31"/>
-      <c r="B102" s="37" t="s">
+      <c r="B102" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="C102" s="37">
+      <c r="C102" s="36">
         <v>3</v>
       </c>
-      <c r="D102" s="36"/>
+      <c r="D102" s="40"/>
       <c r="E102" s="20" t="s">
         <v>205</v>
       </c>
@@ -4131,11 +4137,11 @@
       </c>
       <c r="I102" s="14"/>
     </row>
-    <row r="103" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="31"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="36"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="40"/>
       <c r="E103" s="20" t="s">
         <v>206</v>
       </c>
@@ -4146,11 +4152,11 @@
       </c>
       <c r="I103" s="14"/>
     </row>
-    <row r="104" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="31"/>
-      <c r="B104" s="39"/>
-      <c r="C104" s="39"/>
-      <c r="D104" s="36"/>
+      <c r="B104" s="38"/>
+      <c r="C104" s="38"/>
+      <c r="D104" s="40"/>
       <c r="E104" s="20" t="s">
         <v>207</v>
       </c>
@@ -4161,15 +4167,15 @@
       </c>
       <c r="I104" s="14"/>
     </row>
-    <row r="105" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="31"/>
-      <c r="B105" s="37" t="s">
+      <c r="B105" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C105" s="37">
-        <v>5</v>
-      </c>
-      <c r="D105" s="36"/>
+      <c r="C105" s="36">
+        <v>5</v>
+      </c>
+      <c r="D105" s="40"/>
       <c r="E105" s="20" t="s">
         <v>208</v>
       </c>
@@ -4180,11 +4186,11 @@
       </c>
       <c r="I105" s="14"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="31"/>
-      <c r="B106" s="38"/>
-      <c r="C106" s="38"/>
-      <c r="D106" s="36"/>
+      <c r="B106" s="37"/>
+      <c r="C106" s="37"/>
+      <c r="D106" s="40"/>
       <c r="E106" s="20" t="s">
         <v>209</v>
       </c>
@@ -4195,11 +4201,11 @@
       </c>
       <c r="I106" s="14"/>
     </row>
-    <row r="107" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="31"/>
-      <c r="B107" s="39"/>
-      <c r="C107" s="39"/>
-      <c r="D107" s="36"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="38"/>
+      <c r="D107" s="40"/>
       <c r="E107" s="20" t="s">
         <v>191</v>
       </c>
@@ -4210,15 +4216,15 @@
       </c>
       <c r="I107" s="14"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="31"/>
-      <c r="B108" s="37" t="s">
+      <c r="B108" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C108" s="37">
-        <v>5</v>
-      </c>
-      <c r="D108" s="36"/>
+      <c r="C108" s="36">
+        <v>5</v>
+      </c>
+      <c r="D108" s="40"/>
       <c r="E108" s="20" t="s">
         <v>201</v>
       </c>
@@ -4229,11 +4235,11 @@
       </c>
       <c r="I108" s="14"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="31"/>
-      <c r="B109" s="38"/>
-      <c r="C109" s="38"/>
-      <c r="D109" s="36"/>
+      <c r="B109" s="37"/>
+      <c r="C109" s="37"/>
+      <c r="D109" s="40"/>
       <c r="E109" s="20" t="s">
         <v>202</v>
       </c>
@@ -4244,11 +4250,11 @@
       </c>
       <c r="I109" s="14"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="31"/>
-      <c r="B110" s="39"/>
-      <c r="C110" s="39"/>
-      <c r="D110" s="36"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="38"/>
+      <c r="D110" s="40"/>
       <c r="E110" s="20" t="s">
         <v>203</v>
       </c>
@@ -4259,15 +4265,15 @@
       </c>
       <c r="I110" s="14"/>
     </row>
-    <row r="111" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="31"/>
-      <c r="B111" s="37" t="s">
+      <c r="B111" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C111" s="37">
+      <c r="C111" s="36">
         <v>1</v>
       </c>
-      <c r="D111" s="36"/>
+      <c r="D111" s="40"/>
       <c r="E111" s="20" t="s">
         <v>210</v>
       </c>
@@ -4278,11 +4284,11 @@
       </c>
       <c r="I111" s="14"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="31"/>
-      <c r="B112" s="38"/>
-      <c r="C112" s="38"/>
-      <c r="D112" s="36"/>
+      <c r="B112" s="37"/>
+      <c r="C112" s="37"/>
+      <c r="D112" s="40"/>
       <c r="E112" s="20" t="s">
         <v>211</v>
       </c>
@@ -4293,11 +4299,11 @@
       </c>
       <c r="I112" s="14"/>
     </row>
-    <row r="113" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="32"/>
-      <c r="B113" s="39"/>
-      <c r="C113" s="39"/>
-      <c r="D113" s="36"/>
+      <c r="B113" s="38"/>
+      <c r="C113" s="38"/>
+      <c r="D113" s="40"/>
       <c r="E113" s="20" t="s">
         <v>212</v>
       </c>
@@ -4308,28 +4314,28 @@
       </c>
       <c r="I113" s="14"/>
     </row>
-    <row r="114" spans="1:9" ht="2.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="2.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
-      <c r="D114" s="36"/>
+      <c r="D114" s="40"/>
       <c r="E114" s="21"/>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
     </row>
-    <row r="115" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B115" s="37" t="s">
+      <c r="B115" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="37">
-        <v>5</v>
-      </c>
-      <c r="D115" s="36"/>
+      <c r="C115" s="36">
+        <v>5</v>
+      </c>
+      <c r="D115" s="40"/>
       <c r="E115" s="20" t="s">
         <v>213</v>
       </c>
@@ -4340,11 +4346,11 @@
       </c>
       <c r="I115" s="14"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="31"/>
-      <c r="B116" s="38"/>
-      <c r="C116" s="38"/>
-      <c r="D116" s="36"/>
+      <c r="B116" s="37"/>
+      <c r="C116" s="37"/>
+      <c r="D116" s="40"/>
       <c r="E116" s="20" t="s">
         <v>214</v>
       </c>
@@ -4355,11 +4361,11 @@
       </c>
       <c r="I116" s="14"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="31"/>
-      <c r="B117" s="39"/>
-      <c r="C117" s="39"/>
-      <c r="D117" s="36"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="38"/>
+      <c r="D117" s="40"/>
       <c r="E117" s="20" t="s">
         <v>215</v>
       </c>
@@ -4370,15 +4376,15 @@
       </c>
       <c r="I117" s="14"/>
     </row>
-    <row r="118" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="31"/>
-      <c r="B118" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C118" s="37">
-        <v>5</v>
-      </c>
-      <c r="D118" s="36"/>
+      <c r="B118" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C118" s="36">
+        <v>5</v>
+      </c>
+      <c r="D118" s="40"/>
       <c r="E118" s="20" t="s">
         <v>222</v>
       </c>
@@ -4389,11 +4395,11 @@
       </c>
       <c r="I118" s="14"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="31"/>
-      <c r="B119" s="38"/>
-      <c r="C119" s="38"/>
-      <c r="D119" s="36"/>
+      <c r="B119" s="37"/>
+      <c r="C119" s="37"/>
+      <c r="D119" s="40"/>
       <c r="E119" s="20" t="s">
         <v>224</v>
       </c>
@@ -4404,11 +4410,11 @@
       </c>
       <c r="I119" s="14"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="31"/>
-      <c r="B120" s="39"/>
-      <c r="C120" s="39"/>
-      <c r="D120" s="36"/>
+      <c r="B120" s="38"/>
+      <c r="C120" s="38"/>
+      <c r="D120" s="40"/>
       <c r="E120" s="20" t="s">
         <v>223</v>
       </c>
@@ -4419,15 +4425,15 @@
       </c>
       <c r="I120" s="14"/>
     </row>
-    <row r="121" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="31"/>
-      <c r="B121" s="37" t="s">
+      <c r="B121" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C121" s="37">
-        <v>5</v>
-      </c>
-      <c r="D121" s="36"/>
+      <c r="C121" s="36">
+        <v>5</v>
+      </c>
+      <c r="D121" s="40"/>
       <c r="E121" s="20" t="s">
         <v>216</v>
       </c>
@@ -4438,11 +4444,11 @@
       </c>
       <c r="I121" s="14"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="31"/>
-      <c r="B122" s="38"/>
-      <c r="C122" s="38"/>
-      <c r="D122" s="36"/>
+      <c r="B122" s="37"/>
+      <c r="C122" s="37"/>
+      <c r="D122" s="40"/>
       <c r="E122" s="20" t="s">
         <v>217</v>
       </c>
@@ -4453,11 +4459,11 @@
       </c>
       <c r="I122" s="14"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="31"/>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="36"/>
+      <c r="B123" s="38"/>
+      <c r="C123" s="38"/>
+      <c r="D123" s="40"/>
       <c r="E123" s="20" t="s">
         <v>218</v>
       </c>
@@ -4468,15 +4474,15 @@
       </c>
       <c r="I123" s="14"/>
     </row>
-    <row r="124" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A124" s="31"/>
-      <c r="B124" s="37" t="s">
+      <c r="B124" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C124" s="37">
-        <v>5</v>
-      </c>
-      <c r="D124" s="36"/>
+      <c r="C124" s="36">
+        <v>5</v>
+      </c>
+      <c r="D124" s="40"/>
       <c r="E124" s="20" t="s">
         <v>219</v>
       </c>
@@ -4489,11 +4495,11 @@
         <v>236</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A125" s="31"/>
-      <c r="B125" s="38"/>
-      <c r="C125" s="38"/>
-      <c r="D125" s="36"/>
+      <c r="B125" s="37"/>
+      <c r="C125" s="37"/>
+      <c r="D125" s="40"/>
       <c r="E125" s="20" t="s">
         <v>220</v>
       </c>
@@ -4506,11 +4512,11 @@
         <v>236</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A126" s="31"/>
-      <c r="B126" s="39"/>
-      <c r="C126" s="39"/>
-      <c r="D126" s="36"/>
+      <c r="B126" s="38"/>
+      <c r="C126" s="38"/>
+      <c r="D126" s="40"/>
       <c r="E126" s="20" t="s">
         <v>221</v>
       </c>
@@ -4523,15 +4529,15 @@
         <v>236</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="31"/>
-      <c r="B127" s="37" t="s">
+      <c r="B127" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C127" s="37">
+      <c r="C127" s="36">
         <v>3</v>
       </c>
-      <c r="D127" s="36"/>
+      <c r="D127" s="40"/>
       <c r="E127" s="20" t="s">
         <v>225</v>
       </c>
@@ -4542,11 +4548,11 @@
       </c>
       <c r="I127" s="14"/>
     </row>
-    <row r="128" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="31"/>
-      <c r="B128" s="38"/>
-      <c r="C128" s="38"/>
-      <c r="D128" s="36"/>
+      <c r="B128" s="37"/>
+      <c r="C128" s="37"/>
+      <c r="D128" s="40"/>
       <c r="E128" s="20" t="s">
         <v>226</v>
       </c>
@@ -4557,11 +4563,11 @@
       </c>
       <c r="I128" s="14"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="31"/>
-      <c r="B129" s="39"/>
-      <c r="C129" s="39"/>
-      <c r="D129" s="36"/>
+      <c r="B129" s="38"/>
+      <c r="C129" s="38"/>
+      <c r="D129" s="40"/>
       <c r="E129" s="20" t="s">
         <v>227</v>
       </c>
@@ -4572,15 +4578,15 @@
       </c>
       <c r="I129" s="14"/>
     </row>
-    <row r="130" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A130" s="31"/>
-      <c r="B130" s="37" t="s">
+      <c r="B130" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C130" s="37">
-        <v>5</v>
-      </c>
-      <c r="D130" s="36"/>
+      <c r="C130" s="36">
+        <v>5</v>
+      </c>
+      <c r="D130" s="40"/>
       <c r="E130" s="20" t="s">
         <v>228</v>
       </c>
@@ -4593,11 +4599,11 @@
         <v>237</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A131" s="31"/>
-      <c r="B131" s="38"/>
-      <c r="C131" s="38"/>
-      <c r="D131" s="36"/>
+      <c r="B131" s="37"/>
+      <c r="C131" s="37"/>
+      <c r="D131" s="40"/>
       <c r="E131" s="20" t="s">
         <v>229</v>
       </c>
@@ -4610,11 +4616,11 @@
         <v>237</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A132" s="32"/>
-      <c r="B132" s="39"/>
-      <c r="C132" s="39"/>
-      <c r="D132" s="36"/>
+      <c r="B132" s="38"/>
+      <c r="C132" s="38"/>
+      <c r="D132" s="40"/>
       <c r="E132" s="20" t="s">
         <v>230</v>
       </c>
@@ -4627,28 +4633,28 @@
         <v>237</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
-      <c r="D133" s="36"/>
+      <c r="D133" s="40"/>
       <c r="E133" s="16"/>
       <c r="F133" s="3"/>
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
     </row>
-    <row r="134" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="B134" s="37" t="s">
+      <c r="B134" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C134" s="37">
-        <v>5</v>
-      </c>
-      <c r="D134" s="43"/>
+      <c r="C134" s="36">
+        <v>5</v>
+      </c>
+      <c r="D134" s="41"/>
       <c r="E134" s="20" t="s">
         <v>257</v>
       </c>
@@ -4657,10 +4663,10 @@
       <c r="H134" s="14"/>
       <c r="I134" s="14"/>
     </row>
-    <row r="135" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="31"/>
-      <c r="B135" s="38"/>
-      <c r="C135" s="38"/>
+      <c r="B135" s="37"/>
+      <c r="C135" s="37"/>
       <c r="D135" s="28"/>
       <c r="E135" s="20" t="s">
         <v>199</v>
@@ -4670,10 +4676,10 @@
       <c r="H135" s="14"/>
       <c r="I135" s="14"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="31"/>
-      <c r="B136" s="39"/>
-      <c r="C136" s="39"/>
+      <c r="B136" s="38"/>
+      <c r="C136" s="38"/>
       <c r="D136" s="28"/>
       <c r="E136" s="20" t="s">
         <v>258</v>
@@ -4683,15 +4689,15 @@
       <c r="H136" s="14"/>
       <c r="I136" s="14"/>
     </row>
-    <row r="137" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="31"/>
-      <c r="B137" s="37" t="s">
+      <c r="B137" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C137" s="37">
-        <v>5</v>
-      </c>
-      <c r="D137" s="36"/>
+      <c r="C137" s="36">
+        <v>5</v>
+      </c>
+      <c r="D137" s="40"/>
       <c r="E137" s="20" t="s">
         <v>259</v>
       </c>
@@ -4700,11 +4706,11 @@
       <c r="H137" s="14"/>
       <c r="I137" s="14"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="31"/>
-      <c r="B138" s="38"/>
-      <c r="C138" s="38"/>
-      <c r="D138" s="36"/>
+      <c r="B138" s="37"/>
+      <c r="C138" s="37"/>
+      <c r="D138" s="40"/>
       <c r="E138" s="20" t="s">
         <v>260</v>
       </c>
@@ -4713,11 +4719,11 @@
       <c r="H138" s="14"/>
       <c r="I138" s="14"/>
     </row>
-    <row r="139" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="31"/>
-      <c r="B139" s="39"/>
-      <c r="C139" s="39"/>
-      <c r="D139" s="36"/>
+      <c r="B139" s="38"/>
+      <c r="C139" s="38"/>
+      <c r="D139" s="40"/>
       <c r="E139" s="20" t="s">
         <v>261</v>
       </c>
@@ -4726,15 +4732,15 @@
       <c r="H139" s="14"/>
       <c r="I139" s="14"/>
     </row>
-    <row r="140" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="31"/>
-      <c r="B140" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C140" s="37">
-        <v>5</v>
-      </c>
-      <c r="D140" s="36"/>
+      <c r="B140" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C140" s="36">
+        <v>5</v>
+      </c>
+      <c r="D140" s="40"/>
       <c r="E140" s="20" t="s">
         <v>262</v>
       </c>
@@ -4743,11 +4749,11 @@
       <c r="H140" s="14"/>
       <c r="I140" s="14"/>
     </row>
-    <row r="141" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="31"/>
-      <c r="B141" s="38"/>
-      <c r="C141" s="38"/>
-      <c r="D141" s="36"/>
+      <c r="B141" s="37"/>
+      <c r="C141" s="37"/>
+      <c r="D141" s="40"/>
       <c r="E141" s="20" t="s">
         <v>199</v>
       </c>
@@ -4756,11 +4762,11 @@
       <c r="H141" s="14"/>
       <c r="I141" s="14"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="31"/>
-      <c r="B142" s="39"/>
-      <c r="C142" s="39"/>
-      <c r="D142" s="36"/>
+      <c r="B142" s="38"/>
+      <c r="C142" s="38"/>
+      <c r="D142" s="40"/>
       <c r="E142" s="20" t="s">
         <v>196</v>
       </c>
@@ -4769,15 +4775,15 @@
       <c r="H142" s="14"/>
       <c r="I142" s="14"/>
     </row>
-    <row r="143" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="31"/>
-      <c r="B143" s="37" t="s">
+      <c r="B143" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C143" s="37">
+      <c r="C143" s="36">
         <v>3</v>
       </c>
-      <c r="D143" s="36"/>
+      <c r="D143" s="40"/>
       <c r="E143" s="20" t="s">
         <v>263</v>
       </c>
@@ -4786,11 +4792,11 @@
       <c r="H143" s="14"/>
       <c r="I143" s="14"/>
     </row>
-    <row r="144" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="31"/>
-      <c r="B144" s="38"/>
-      <c r="C144" s="38"/>
-      <c r="D144" s="36"/>
+      <c r="B144" s="37"/>
+      <c r="C144" s="37"/>
+      <c r="D144" s="40"/>
       <c r="E144" s="20" t="s">
         <v>199</v>
       </c>
@@ -4799,11 +4805,11 @@
       <c r="H144" s="14"/>
       <c r="I144" s="14"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="31"/>
-      <c r="B145" s="39"/>
-      <c r="C145" s="39"/>
-      <c r="D145" s="36"/>
+      <c r="B145" s="38"/>
+      <c r="C145" s="38"/>
+      <c r="D145" s="40"/>
       <c r="E145" s="20" t="s">
         <v>196</v>
       </c>
@@ -4812,15 +4818,15 @@
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="31"/>
-      <c r="B146" s="37" t="s">
+      <c r="B146" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C146" s="37">
+      <c r="C146" s="36">
         <v>2</v>
       </c>
-      <c r="D146" s="36"/>
+      <c r="D146" s="40"/>
       <c r="E146" s="20" t="s">
         <v>248</v>
       </c>
@@ -4829,11 +4835,11 @@
       <c r="H146" s="14"/>
       <c r="I146" s="14"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="31"/>
-      <c r="B147" s="38"/>
-      <c r="C147" s="38"/>
-      <c r="D147" s="36"/>
+      <c r="B147" s="37"/>
+      <c r="C147" s="37"/>
+      <c r="D147" s="40"/>
       <c r="E147" s="20" t="s">
         <v>249</v>
       </c>
@@ -4842,11 +4848,11 @@
       <c r="H147" s="14"/>
       <c r="I147" s="14"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="31"/>
-      <c r="B148" s="39"/>
-      <c r="C148" s="39"/>
-      <c r="D148" s="36"/>
+      <c r="B148" s="38"/>
+      <c r="C148" s="38"/>
+      <c r="D148" s="40"/>
       <c r="E148" s="20" t="s">
         <v>250</v>
       </c>
@@ -4855,15 +4861,15 @@
       <c r="H148" s="14"/>
       <c r="I148" s="14"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="31"/>
-      <c r="B149" s="37" t="s">
+      <c r="B149" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C149" s="37">
+      <c r="C149" s="36">
         <v>2</v>
       </c>
-      <c r="D149" s="36"/>
+      <c r="D149" s="40"/>
       <c r="E149" s="20" t="s">
         <v>248</v>
       </c>
@@ -4872,11 +4878,11 @@
       <c r="H149" s="14"/>
       <c r="I149" s="14"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="31"/>
-      <c r="B150" s="38"/>
-      <c r="C150" s="38"/>
-      <c r="D150" s="36"/>
+      <c r="B150" s="37"/>
+      <c r="C150" s="37"/>
+      <c r="D150" s="40"/>
       <c r="E150" s="20" t="s">
         <v>249</v>
       </c>
@@ -4885,11 +4891,11 @@
       <c r="H150" s="14"/>
       <c r="I150" s="14"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="31"/>
-      <c r="B151" s="39"/>
-      <c r="C151" s="39"/>
-      <c r="D151" s="36"/>
+      <c r="B151" s="38"/>
+      <c r="C151" s="38"/>
+      <c r="D151" s="40"/>
       <c r="E151" s="20" t="s">
         <v>250</v>
       </c>
@@ -4898,15 +4904,15 @@
       <c r="H151" s="14"/>
       <c r="I151" s="14"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="31"/>
-      <c r="B152" s="37" t="s">
+      <c r="B152" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C152" s="37">
+      <c r="C152" s="36">
         <v>1</v>
       </c>
-      <c r="D152" s="36"/>
+      <c r="D152" s="40"/>
       <c r="E152" s="20" t="s">
         <v>248</v>
       </c>
@@ -4915,11 +4921,11 @@
       <c r="H152" s="14"/>
       <c r="I152" s="14"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="31"/>
-      <c r="B153" s="38"/>
-      <c r="C153" s="38"/>
-      <c r="D153" s="36"/>
+      <c r="B153" s="37"/>
+      <c r="C153" s="37"/>
+      <c r="D153" s="40"/>
       <c r="E153" s="20" t="s">
         <v>249</v>
       </c>
@@ -4928,11 +4934,11 @@
       <c r="H153" s="14"/>
       <c r="I153" s="14"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="31"/>
-      <c r="B154" s="39"/>
-      <c r="C154" s="39"/>
-      <c r="D154" s="36"/>
+      <c r="B154" s="38"/>
+      <c r="C154" s="38"/>
+      <c r="D154" s="40"/>
       <c r="E154" s="20" t="s">
         <v>250</v>
       </c>
@@ -4941,15 +4947,15 @@
       <c r="H154" s="14"/>
       <c r="I154" s="14"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="31"/>
-      <c r="B155" s="37" t="s">
+      <c r="B155" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C155" s="37">
-        <v>5</v>
-      </c>
-      <c r="D155" s="36"/>
+      <c r="C155" s="36">
+        <v>5</v>
+      </c>
+      <c r="D155" s="40"/>
       <c r="E155" s="20" t="s">
         <v>248</v>
       </c>
@@ -4958,11 +4964,11 @@
       <c r="H155" s="14"/>
       <c r="I155" s="14"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="31"/>
-      <c r="B156" s="38"/>
-      <c r="C156" s="38"/>
-      <c r="D156" s="36"/>
+      <c r="B156" s="37"/>
+      <c r="C156" s="37"/>
+      <c r="D156" s="40"/>
       <c r="E156" s="20" t="s">
         <v>249</v>
       </c>
@@ -4971,11 +4977,11 @@
       <c r="H156" s="14"/>
       <c r="I156" s="14"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="31"/>
-      <c r="B157" s="39"/>
-      <c r="C157" s="39"/>
-      <c r="D157" s="36"/>
+      <c r="B157" s="38"/>
+      <c r="C157" s="38"/>
+      <c r="D157" s="40"/>
       <c r="E157" s="20" t="s">
         <v>250</v>
       </c>
@@ -4986,6 +4992,86 @@
     </row>
   </sheetData>
   <mergeCells count="104">
+    <mergeCell ref="D137:D157"/>
+    <mergeCell ref="A134:A157"/>
+    <mergeCell ref="B146:B148"/>
+    <mergeCell ref="B149:B151"/>
+    <mergeCell ref="B152:B154"/>
+    <mergeCell ref="B155:B157"/>
+    <mergeCell ref="C134:C136"/>
+    <mergeCell ref="C137:C139"/>
+    <mergeCell ref="C140:C142"/>
+    <mergeCell ref="C143:C145"/>
+    <mergeCell ref="C146:C148"/>
+    <mergeCell ref="C149:C151"/>
+    <mergeCell ref="C152:C154"/>
+    <mergeCell ref="C155:C157"/>
+    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="B140:B142"/>
+    <mergeCell ref="B143:B145"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A76:A89"/>
+    <mergeCell ref="A91:A113"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="A4:A74"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="A115:A132"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="C63:C65"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="B98:B101"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C85:C87"/>
+    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="C76:C78"/>
     <mergeCell ref="B91:B94"/>
     <mergeCell ref="D2:D134"/>
     <mergeCell ref="B127:B129"/>
@@ -5010,86 +5096,6 @@
     <mergeCell ref="C98:C101"/>
     <mergeCell ref="C95:C97"/>
     <mergeCell ref="B105:B107"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="B98:B101"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="B85:B87"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="A115:A132"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="C63:C65"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A76:A89"/>
-    <mergeCell ref="A91:A113"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="A4:A74"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="C85:C87"/>
-    <mergeCell ref="C82:C84"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="D137:D157"/>
-    <mergeCell ref="A134:A157"/>
-    <mergeCell ref="B146:B148"/>
-    <mergeCell ref="B149:B151"/>
-    <mergeCell ref="B152:B154"/>
-    <mergeCell ref="B155:B157"/>
-    <mergeCell ref="C134:C136"/>
-    <mergeCell ref="C137:C139"/>
-    <mergeCell ref="C140:C142"/>
-    <mergeCell ref="C143:C145"/>
-    <mergeCell ref="C146:C148"/>
-    <mergeCell ref="C149:C151"/>
-    <mergeCell ref="C152:C154"/>
-    <mergeCell ref="C155:C157"/>
-    <mergeCell ref="B134:B136"/>
-    <mergeCell ref="B137:B139"/>
-    <mergeCell ref="B140:B142"/>
-    <mergeCell ref="B143:B145"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>